<commit_message>
Finalised exports - excluding HSI
</commit_message>
<xml_diff>
--- a/scripts/modeltools/exports/Scenario_Results.xlsx
+++ b/scripts/modeltools/exports/Scenario_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\CDM\scripts\modeltools\exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B69CC9A-997E-4FF8-A3FF-44ACA9201CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7E56EE-1819-41C3-AB95-7A9EED369E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AB718105-107C-43D2-99B7-2FF2B3DDDF7D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="173">
   <si>
     <t>Critical CPS</t>
   </si>
@@ -312,9 +312,6 @@
     <t>Salt Creek flow is &gt;3 ML/day and CSL is &gt;+0.4 m AHD or Salt Creek flow &gt;2 ML/day and CSL is &gt;+0.8 m AHD</t>
   </si>
   <si>
-    <t>% of days where Salt Creek flow is &gt;3 ML/day and average CSL is &gt;+0.4 m AHD or Salt Creek flow is &gt;2 ML/day and average CSL is &gt;+0.8 m AHD</t>
-  </si>
-  <si>
     <t>Export 8</t>
   </si>
   <si>
@@ -337,9 +334,6 @@
   </si>
   <si>
     <t>6.5 mg/L</t>
-  </si>
-  <si>
-    <t>ME, CNL</t>
   </si>
   <si>
     <t>Average daily area (HA) that minimum DO is ≥6.5 mg/L</t>
@@ -652,6 +646,18 @@
   </si>
   <si>
     <t>HSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of days where Salt Creek flow is &gt;3 ML/day and average CSL is &gt;+0.4 m AHD </t>
+  </si>
+  <si>
+    <t>% of days whereSalt Creek flow is &gt;2 ML/day and average CSL is &gt;+0.8 m AHD</t>
+  </si>
+  <si>
+    <t>% of days where Salt Creek flow is &gt;3 ML/day and average CSL is &gt;+0.4 m AHD</t>
+  </si>
+  <si>
+    <t>% of days where Salt Creek flow is &gt;2 ML/day and average CSL is &gt;+0.8 m AHD</t>
   </si>
 </sst>
 </file>
@@ -1150,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3323FCED-6F7F-45C8-A947-57EDCFA88034}">
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83:XFD83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="44.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1193,42 +1199,42 @@
         <v>5</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="K1" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="10" t="s">
         <v>149</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>152</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>154</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
@@ -1239,25 +1245,25 @@
     </row>
     <row r="3" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>152</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>154</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>74</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -1268,16 +1274,16 @@
     </row>
     <row r="4" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>22</v>
@@ -1286,7 +1292,7 @@
         <v>14</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -1297,16 +1303,16 @@
     </row>
     <row r="5" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>22</v>
@@ -1315,7 +1321,7 @@
         <v>74</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -1326,16 +1332,16 @@
     </row>
     <row r="6" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>22</v>
@@ -1344,7 +1350,7 @@
         <v>14</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -1355,16 +1361,16 @@
     </row>
     <row r="7" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>22</v>
@@ -1373,7 +1379,7 @@
         <v>74</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -1384,16 +1390,16 @@
     </row>
     <row r="8" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>24</v>
@@ -1402,7 +1408,7 @@
         <v>14</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
@@ -1413,16 +1419,16 @@
     </row>
     <row r="9" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>24</v>
@@ -1431,7 +1437,7 @@
         <v>74</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -1442,16 +1448,16 @@
     </row>
     <row r="10" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>25</v>
@@ -1460,7 +1466,7 @@
         <v>14</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
@@ -1471,16 +1477,16 @@
     </row>
     <row r="11" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>25</v>
@@ -1489,7 +1495,7 @@
         <v>74</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -1500,16 +1506,16 @@
     </row>
     <row r="12" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>25</v>
@@ -1518,7 +1524,7 @@
         <v>14</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
@@ -1529,16 +1535,16 @@
     </row>
     <row r="13" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>25</v>
@@ -1547,7 +1553,7 @@
         <v>74</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
@@ -1558,16 +1564,16 @@
     </row>
     <row r="14" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>25</v>
@@ -1576,7 +1582,7 @@
         <v>14</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -1587,16 +1593,16 @@
     </row>
     <row r="15" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>25</v>
@@ -1605,7 +1611,7 @@
         <v>74</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -1616,25 +1622,25 @@
     </row>
     <row r="16" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>74</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -1645,25 +1651,25 @@
     </row>
     <row r="17" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
@@ -1674,25 +1680,25 @@
     </row>
     <row r="18" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>76</v>
       </c>
       <c r="C18" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>165</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>167</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>14</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -1703,25 +1709,25 @@
     </row>
     <row r="19" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>76</v>
       </c>
       <c r="C19" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>165</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>167</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>74</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -1732,25 +1738,25 @@
     </row>
     <row r="20" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>76</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
@@ -1761,25 +1767,25 @@
     </row>
     <row r="21" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>76</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>74</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -2062,7 +2068,7 @@
         <v>23</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -2090,7 +2096,7 @@
         <v>23</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -2118,7 +2124,7 @@
         <v>23</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -2146,7 +2152,7 @@
         <v>28</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -2174,7 +2180,7 @@
         <v>28</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -2216,7 +2222,7 @@
         <v>28</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H38" s="16">
         <v>39.570500000000003</v>
@@ -2254,7 +2260,7 @@
         <v>28</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H39" s="16">
         <v>55.456800000000001</v>
@@ -2292,7 +2298,7 @@
         <v>28</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H40" s="16">
         <v>106.744</v>
@@ -2330,7 +2336,7 @@
         <v>28</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H41" s="16">
         <v>85.593400000000003</v>
@@ -2368,7 +2374,7 @@
         <v>28</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H42" s="16">
         <v>184.9444</v>
@@ -2406,7 +2412,7 @@
         <v>28</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H43" s="16">
         <v>166.74610000000001</v>
@@ -2458,7 +2464,7 @@
         <v>28</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H45" s="16">
         <v>5.0000000000000001E-4</v>
@@ -2496,7 +2502,7 @@
         <v>28</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H46" s="16">
         <v>6.7299999999999999E-2</v>
@@ -3306,7 +3312,7 @@
     </row>
     <row r="71" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B71" s="15" t="s">
         <v>46</v>
@@ -3324,7 +3330,7 @@
         <v>74</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>92</v>
+        <v>169</v>
       </c>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
@@ -3334,25 +3340,25 @@
     </row>
     <row r="72" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B72" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C72" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C72" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D72" s="14" t="s">
+      <c r="D72" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E72" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F72" s="14" t="s">
+      <c r="E72" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="G72" s="14" t="s">
-        <v>92</v>
+      <c r="G72" s="15" t="s">
+        <v>170</v>
       </c>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
@@ -3361,13 +3367,27 @@
       <c r="L72" s="3"/>
     </row>
     <row r="73" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
+      <c r="A73" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G73" s="14" t="s">
+        <v>171</v>
+      </c>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
@@ -3376,352 +3396,372 @@
     </row>
     <row r="74" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E74" s="14" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="G74" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="H74" s="16">
-        <v>2587.1439999999998</v>
-      </c>
-      <c r="I74" s="16">
-        <v>2997.8051</v>
-      </c>
-      <c r="J74" s="16">
-        <v>2589.886</v>
-      </c>
-      <c r="K74">
-        <v>2532.9160000000002</v>
-      </c>
-      <c r="L74">
-        <v>3216.6961999999999</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
     </row>
     <row r="75" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B75" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C75" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D75" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="E75" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F75" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G75" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="H75" s="16">
-        <v>3371.7710000000002</v>
-      </c>
-      <c r="I75" s="16">
-        <v>3831.4337</v>
-      </c>
-      <c r="J75" s="16">
-        <v>3374.3874000000001</v>
-      </c>
-      <c r="K75">
-        <v>3309.9659999999999</v>
-      </c>
-      <c r="L75">
-        <v>4075.6783999999998</v>
-      </c>
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
     </row>
     <row r="76" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B76" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C76" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D76" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E76" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="G76" s="15" t="s">
-        <v>102</v>
+        <v>105</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E76" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F76" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G76" s="14" t="s">
+        <v>95</v>
       </c>
       <c r="H76" s="16">
-        <v>7927.5046000000002</v>
+        <v>2587.1439999999998</v>
       </c>
       <c r="I76" s="16">
-        <v>6644.1750000000002</v>
+        <v>2997.8051</v>
       </c>
       <c r="J76" s="16">
-        <v>7927.5046000000002</v>
+        <v>2589.886</v>
       </c>
       <c r="K76">
-        <v>8211.9550999999992</v>
+        <v>2532.9160000000002</v>
       </c>
       <c r="L76">
-        <v>6186.6490999999996</v>
+        <v>3216.6961999999999</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B77" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C77" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D77" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E77" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F77" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="G77" s="14" t="s">
-        <v>102</v>
+        <v>105</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F77" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G77" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="H77" s="16">
-        <v>5574.6918999999998</v>
+        <v>3371.7710000000002</v>
       </c>
       <c r="I77" s="16">
-        <v>3135.7692999999999</v>
+        <v>3831.4337</v>
       </c>
       <c r="J77" s="16">
-        <v>5579.4000999999998</v>
+        <v>3374.3874000000001</v>
       </c>
       <c r="K77">
-        <v>6517.7440999999999</v>
+        <v>3309.9659999999999</v>
       </c>
       <c r="L77">
-        <v>2117.8793000000001</v>
+        <v>4075.6783999999998</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B78" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C78" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D78" s="15" t="s">
         <v>99</v>
-      </c>
-      <c r="D78" s="15" t="s">
-        <v>103</v>
       </c>
       <c r="E78" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F78" s="15" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G78" s="15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H78" s="16">
-        <v>10745.921700000001</v>
+        <v>7927.5046000000002</v>
       </c>
       <c r="I78" s="16">
-        <v>10224.4136</v>
+        <v>6644.1750000000002</v>
       </c>
       <c r="J78" s="16">
-        <v>10745.921700000001</v>
+        <v>7927.5046000000002</v>
       </c>
       <c r="K78">
-        <v>10844.952499999999</v>
+        <v>8211.9550999999992</v>
       </c>
       <c r="L78">
-        <v>9761.7330000000002</v>
+        <v>6186.6490999999996</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B79" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C79" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D79" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="D79" s="14" t="s">
-        <v>103</v>
       </c>
       <c r="E79" s="14" t="s">
         <v>13</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H79" s="16">
-        <v>9925.2494999999999</v>
+        <v>5574.6918999999998</v>
       </c>
       <c r="I79" s="16">
-        <v>5573.0412999999999</v>
+        <v>3135.7692999999999</v>
       </c>
       <c r="J79" s="16">
-        <v>9930.7656000000006</v>
+        <v>5579.4000999999998</v>
       </c>
       <c r="K79">
-        <v>10260.0533</v>
+        <v>6517.7440999999999</v>
       </c>
       <c r="L79">
-        <v>4370.9804999999997</v>
+        <v>2117.8793000000001</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B80" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D80" s="15" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="E80" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F80" s="15" t="s">
-        <v>101</v>
+        <v>42</v>
       </c>
       <c r="G80" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-      <c r="K80" s="3"/>
-      <c r="L80" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="H80" s="16">
+        <v>7927.5046000000002</v>
+      </c>
+      <c r="I80" s="16">
+        <v>6644.1750000000002</v>
+      </c>
+      <c r="J80" s="16">
+        <v>7927.5046000000002</v>
+      </c>
+      <c r="K80">
+        <v>8211.9550999999992</v>
+      </c>
+      <c r="L80">
+        <v>6186.6490999999996</v>
+      </c>
     </row>
     <row r="81" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B81" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="E81" s="14" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G81" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="H81" s="3"/>
-      <c r="I81" s="3"/>
-      <c r="J81" s="3"/>
-      <c r="K81" s="3"/>
-      <c r="L81" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="H81" s="16">
+        <v>5574.6918999999998</v>
+      </c>
+      <c r="I81" s="16">
+        <v>3135.7692999999999</v>
+      </c>
+      <c r="J81" s="16">
+        <v>5579.4000999999998</v>
+      </c>
+      <c r="K81">
+        <v>6517.7440999999999</v>
+      </c>
+      <c r="L81">
+        <v>2117.8793000000001</v>
+      </c>
     </row>
     <row r="82" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B82" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D82" s="15" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="E82" s="15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F82" s="15" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="G82" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
-      <c r="K82" s="3"/>
-      <c r="L82" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="H82" s="16">
+        <v>10745.921700000001</v>
+      </c>
+      <c r="I82" s="16">
+        <v>10224.4136</v>
+      </c>
+      <c r="J82" s="16">
+        <v>10745.921700000001</v>
+      </c>
+      <c r="K82">
+        <v>10844.952499999999</v>
+      </c>
+      <c r="L82">
+        <v>9761.7330000000002</v>
+      </c>
     </row>
     <row r="83" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B83" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="E83" s="14" t="s">
         <v>13</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="G83" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="H83" s="3"/>
-      <c r="I83" s="3"/>
-      <c r="J83" s="3"/>
-      <c r="K83" s="3"/>
-      <c r="L83" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="H83" s="16">
+        <v>9925.2494999999999</v>
+      </c>
+      <c r="I83" s="16">
+        <v>5573.0412999999999</v>
+      </c>
+      <c r="J83" s="16">
+        <v>9930.7656000000006</v>
+      </c>
+      <c r="K83">
+        <v>10260.0533</v>
+      </c>
+      <c r="L83">
+        <v>4370.9804999999997</v>
+      </c>
     </row>
     <row r="84" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
+      <c r="A84" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E84" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G84" s="15" t="s">
+        <v>104</v>
+      </c>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
@@ -3730,50 +3770,54 @@
     </row>
     <row r="85" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B85" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D85" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="E85" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F85" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G85" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="H85" s="16">
-        <v>6.7295999999999996</v>
-      </c>
-      <c r="I85" s="16">
-        <v>18.209299999999999</v>
-      </c>
-      <c r="J85" s="16">
-        <v>6.7733999999999996</v>
-      </c>
-      <c r="K85">
-        <v>3.5562999999999998</v>
-      </c>
-      <c r="L85">
-        <v>7.6878000000000002</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E85" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G85" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="3"/>
     </row>
     <row r="86" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="3"/>
+      <c r="A86" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E86" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" s="14" t="s">
+        <v>104</v>
+      </c>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
@@ -3782,25 +3826,25 @@
     </row>
     <row r="87" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B87" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C87" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D87" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="E87" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="F87" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="G87" s="14" t="s">
-        <v>113</v>
+        <v>105</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E87" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F87" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G87" s="15" t="s">
+        <v>104</v>
       </c>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
@@ -3810,25 +3854,25 @@
     </row>
     <row r="88" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="D88" s="15" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="E88" s="15" t="s">
-        <v>112</v>
+        <v>13</v>
       </c>
       <c r="F88" s="15" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="G88" s="15" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
@@ -3838,25 +3882,25 @@
     </row>
     <row r="89" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
       <c r="E89" s="14" t="s">
-        <v>117</v>
+        <v>13</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="G89" s="14" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
@@ -3865,27 +3909,13 @@
       <c r="L89" s="3"/>
     </row>
     <row r="90" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B90" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C90" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D90" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="E90" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="F90" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="G90" s="15" t="s">
-        <v>120</v>
-      </c>
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
@@ -3894,31 +3924,41 @@
     </row>
     <row r="91" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B91" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D91" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="E91" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F91" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="G91" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="H91" s="3"/>
-      <c r="I91" s="3"/>
-      <c r="J91" s="3"/>
-      <c r="K91" s="3"/>
-      <c r="L91" s="3"/>
+        <v>108</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C91" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D91" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E91" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F91" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G91" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H91" s="16">
+        <v>6.7295999999999996</v>
+      </c>
+      <c r="I91" s="16">
+        <v>18.209299999999999</v>
+      </c>
+      <c r="J91" s="16">
+        <v>6.7733999999999996</v>
+      </c>
+      <c r="K91">
+        <v>3.5562999999999998</v>
+      </c>
+      <c r="L91">
+        <v>7.6878000000000002</v>
+      </c>
     </row>
     <row r="92" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
@@ -3936,25 +3976,25 @@
     </row>
     <row r="93" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B93" s="14" t="s">
         <v>58</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="E93" s="14" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="F93" s="14" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="G93" s="14" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
@@ -3964,25 +4004,25 @@
     </row>
     <row r="94" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B94" s="15" t="s">
         <v>58</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="D94" s="15" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="E94" s="15" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="F94" s="15" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="G94" s="15" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
@@ -3992,25 +4032,25 @@
     </row>
     <row r="95" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B95" s="14" t="s">
         <v>58</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E95" s="14" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F95" s="14" t="s">
         <v>74</v>
       </c>
       <c r="G95" s="14" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
@@ -4020,25 +4060,25 @@
     </row>
     <row r="96" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B96" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B96" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C96" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D96" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="E96" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="F96" s="14" t="s">
+      <c r="C96" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E96" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F96" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="G96" s="14" t="s">
-        <v>131</v>
+      <c r="G96" s="15" t="s">
+        <v>118</v>
       </c>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
@@ -4047,13 +4087,27 @@
       <c r="L96" s="3"/>
     </row>
     <row r="97" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="3"/>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
-      <c r="G97" s="3"/>
+      <c r="A97" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C97" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="E97" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F97" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="G97" s="15" t="s">
+        <v>120</v>
+      </c>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
@@ -4061,27 +4115,13 @@
       <c r="L97" s="3"/>
     </row>
     <row r="98" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B98" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C98" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D98" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="E98" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="F98" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="G98" s="14" t="s">
-        <v>133</v>
-      </c>
+      <c r="A98" s="3"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
@@ -4089,13 +4129,27 @@
       <c r="L98" s="3"/>
     </row>
     <row r="99" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="3"/>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="3"/>
-      <c r="F99" s="3"/>
-      <c r="G99" s="3"/>
+      <c r="A99" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C99" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D99" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E99" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F99" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G99" s="14" t="s">
+        <v>123</v>
+      </c>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
@@ -4104,153 +4158,293 @@
     </row>
     <row r="100" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B100" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C100" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D100" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E100" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F100" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="G100" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="H100" s="16">
-        <v>3.8160599999999998</v>
-      </c>
-      <c r="I100" s="16">
-        <v>3.92754</v>
-      </c>
-      <c r="J100" s="16">
-        <v>3.8160599999999998</v>
-      </c>
-      <c r="K100">
-        <v>4.0979400000000004</v>
-      </c>
-      <c r="L100">
-        <v>3.9694199999999999</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="B100" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C100" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="E100" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F100" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G100" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="H100" s="3"/>
+      <c r="I100" s="3"/>
+      <c r="J100" s="3"/>
+      <c r="K100" s="3"/>
+      <c r="L100" s="3"/>
     </row>
     <row r="101" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B101" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C101" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="D101" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="E101" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F101" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G101" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="H101" s="16">
-        <v>9.0234000000000005</v>
-      </c>
-      <c r="I101" s="16">
-        <v>11.540190000000001</v>
-      </c>
-      <c r="J101" s="16">
-        <v>9.0192800000000002</v>
-      </c>
-      <c r="K101">
-        <v>8.4071800000000003</v>
-      </c>
-      <c r="L101">
-        <v>13.09352</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C101" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E101" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F101" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G101" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+      <c r="L101" s="3"/>
     </row>
     <row r="102" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E102" s="14" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="F102" s="14" t="s">
         <v>74</v>
       </c>
       <c r="G102" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="H102" s="3"/>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
+    </row>
+    <row r="103" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+      <c r="I103" s="3"/>
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="3"/>
+    </row>
+    <row r="104" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B104" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C104" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D104" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E104" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F104" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G104" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="H104" s="3"/>
+      <c r="I104" s="3"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+    </row>
+    <row r="105" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3"/>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
+      <c r="I105" s="3"/>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="3"/>
+    </row>
+    <row r="106" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C106" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D106" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E106" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F106" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="G106" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H106" s="16">
+        <v>3.8160599999999998</v>
+      </c>
+      <c r="I106" s="16">
+        <v>3.92754</v>
+      </c>
+      <c r="J106" s="16">
+        <v>3.8160599999999998</v>
+      </c>
+      <c r="K106">
+        <v>4.0979400000000004</v>
+      </c>
+      <c r="L106">
+        <v>3.9694199999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B107" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C107" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D107" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E107" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F107" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G107" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="H107" s="16">
+        <v>9.0234000000000005</v>
+      </c>
+      <c r="I107" s="16">
+        <v>11.540190000000001</v>
+      </c>
+      <c r="J107" s="16">
+        <v>9.0192800000000002</v>
+      </c>
+      <c r="K107">
+        <v>8.4071800000000003</v>
+      </c>
+      <c r="L107">
+        <v>13.09352</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B108" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C108" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D108" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="H102" s="16">
+      <c r="E108" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F108" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G108" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H108" s="16">
         <v>24.45495</v>
       </c>
-      <c r="I102" s="16">
+      <c r="I108" s="16">
         <v>32.115299999999998</v>
       </c>
-      <c r="J102" s="16">
+      <c r="J108" s="16">
         <v>24.45495</v>
       </c>
-      <c r="K102">
+      <c r="K108">
         <v>21.699919999999999</v>
       </c>
-      <c r="L102">
+      <c r="L108">
         <v>34.323300000000003</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B103" s="15" t="s">
+    <row r="109" spans="1:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B109" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C103" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="D103" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="E103" s="15" t="s">
+      <c r="C109" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D109" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E109" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F103" s="15" t="s">
+      <c r="F109" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="G103" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="H103" s="16">
+      <c r="G109" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="H109" s="16">
         <v>45.18683</v>
       </c>
-      <c r="I103" s="16">
+      <c r="I109" s="16">
         <v>62.286200000000001</v>
       </c>
-      <c r="J103" s="16">
+      <c r="J109" s="16">
         <v>45.276060000000001</v>
       </c>
-      <c r="K103">
+      <c r="K109">
         <v>40.492989999999999</v>
       </c>
-      <c r="L103">
+      <c r="L109">
         <v>66.184269999999998</v>
       </c>
     </row>

</xml_diff>